<commit_message>
Add routing for SPA
</commit_message>
<xml_diff>
--- a/AngularWithC#.xlsx
+++ b/AngularWithC#.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="47">
   <si>
     <t>Tools for developing</t>
   </si>
@@ -149,6 +149,15 @@
   </si>
   <si>
     <t>ESLint</t>
+  </si>
+  <si>
+    <t>Angular commands</t>
+  </si>
+  <si>
+    <t>ng g guard auth --skipTests</t>
+  </si>
+  <si>
+    <t>Generate guard</t>
   </si>
 </sst>
 </file>
@@ -534,10 +543,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -744,6 +753,19 @@
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" t="s">
+        <v>45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Register Form - ReactiveForm
</commit_message>
<xml_diff>
--- a/AngularWithC#.xlsx
+++ b/AngularWithC#.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
   <si>
     <t>Tools for developing</t>
   </si>
@@ -173,6 +173,12 @@
   </si>
   <si>
     <t>The best way to quickly integrate Bootstrap 3 or Bootstrap 4 Components with Angular</t>
+  </si>
+  <si>
+    <t>ng2-file-upload</t>
+  </si>
+  <si>
+    <t>Easy to use Angular2 directives for files upload (demo)</t>
   </si>
 </sst>
 </file>
@@ -558,16 +564,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="55.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="60.42578125" customWidth="1"/>
     <col min="3" max="3" width="74.140625" customWidth="1"/>
     <col min="4" max="4" width="32.42578125" bestFit="1" customWidth="1"/>
   </cols>
@@ -586,221 +592,232 @@
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="A3" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" t="s">
         <v>51</v>
-      </c>
-      <c r="C4" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
         <v>49</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C6" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B8" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>6</v>
-      </c>
-      <c r="C8" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
+    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D14" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="2"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C18" t="s">
-        <v>27</v>
-      </c>
-      <c r="D18" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="C19" t="s">
-        <v>40</v>
+        <v>27</v>
+      </c>
+      <c r="D19" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C20" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="B21" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B23" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
-        <v>8</v>
-      </c>
-      <c r="C24" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>12</v>
-      </c>
-      <c r="C25" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>35</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B29" t="s">
         <v>36</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C29" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
-        <v>17</v>
-      </c>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>46</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B37" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
TimeAgo Pipe And Antion Filters
</commit_message>
<xml_diff>
--- a/AngularWithC#.xlsx
+++ b/AngularWithC#.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
   <si>
     <t>Tools for developing</t>
   </si>
@@ -179,6 +179,12 @@
   </si>
   <si>
     <t>Easy to use Angular2 directives for files upload (demo)</t>
+  </si>
+  <si>
+    <t>ngx-timeago</t>
+  </si>
+  <si>
+    <t>Live updating timestamps in Angular 6+.</t>
   </si>
 </sst>
 </file>
@@ -564,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -621,203 +627,211 @@
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
+      <c r="B7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="2" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-      <c r="C9" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B10" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B14" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
+    <row r="15" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="B15" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="D15" s="2"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C19" t="s">
-        <v>27</v>
-      </c>
-      <c r="D19" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
-        <v>39</v>
+        <v>25</v>
       </c>
       <c r="C20" t="s">
-        <v>40</v>
+        <v>27</v>
+      </c>
+      <c r="D20" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C21" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B22" s="2"/>
+      <c r="B22" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="1" t="s">
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B24" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
-        <v>10</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
         <v>8</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C27" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+    <row r="28" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
         <v>12</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C28" s="2" t="s">
         <v>13</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
-        <v>35</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
+        <v>35</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B30" t="s">
         <v>36</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C30" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
-        <v>16</v>
-      </c>
+      <c r="B32" s="3"/>
+      <c r="C32" s="3"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>46</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>45</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add sorting and filtering
</commit_message>
<xml_diff>
--- a/AngularWithC#.xlsx
+++ b/AngularWithC#.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="7515"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="57">
   <si>
     <t>Tools for developing</t>
   </si>
@@ -185,12 +185,15 @@
   </si>
   <si>
     <t>Live updating timestamps in Angular 6+.</t>
+  </si>
+  <si>
+    <t>Add angular snippets</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -326,7 +329,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -361,7 +364,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -573,7 +576,7 @@
   <dimension ref="A1:D38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -661,6 +664,9 @@
       </c>
       <c r="C11" t="s">
         <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>